<commit_message>
enny06 20190514 09.07 DB Greebel Backup Menu
</commit_message>
<xml_diff>
--- a/doc/GREEBEL20190430.xlsx
+++ b/doc/GREEBEL20190430.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="30" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="206">
   <si>
     <t>ItemCode</t>
   </si>
@@ -61,9 +61,6 @@
   </si>
   <si>
     <t>ItemMainGroupId</t>
-  </si>
-  <si>
-    <t>LastBuyingPrice</t>
   </si>
   <si>
     <t>decimal</t>
@@ -642,8 +639,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -821,14 +818,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -836,6 +833,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2625,6 +2627,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2659,6 +2662,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2834,50 +2838,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G200"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G199"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A159" sqref="A159"/>
+      <selection pane="bottomLeft" activeCell="A96" sqref="A96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.5703125" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="14" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="14"/>
     <col min="4" max="4" width="13.28515625" style="14" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" style="14" customWidth="1"/>
     <col min="7" max="7" width="100.7109375" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="45.75" customHeight="1">
+    <row r="1" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -2886,9 +2890,9 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
@@ -2897,83 +2901,83 @@
       <c r="F3" s="7"/>
       <c r="G3" s="8"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="7"/>
       <c r="D4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F4" s="7"/>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F6" s="7">
         <v>100</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F7" s="7">
         <v>0</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="8"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -2981,10 +2985,10 @@
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -2992,10 +2996,10 @@
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -3004,9 +3008,9 @@
       <c r="F10" s="7"/>
       <c r="G10" s="8"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -3014,42 +3018,42 @@
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="8"/>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -3058,7 +3062,7 @@
       <c r="F14" s="7"/>
       <c r="G14" s="8"/>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -3067,9 +3071,9 @@
       <c r="F15" s="7"/>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -3077,40 +3081,40 @@
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
       <c r="G16" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="8"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -3119,9 +3123,9 @@
       <c r="F19" s="7"/>
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -3129,55 +3133,55 @@
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
       <c r="G20" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="8" t="s">
-        <v>79</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
       <c r="G21" s="8"/>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
       <c r="G22" s="8"/>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="7"/>
       <c r="D23" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="G23" s="8"/>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -3186,9 +3190,9 @@
       <c r="F24" s="7"/>
       <c r="G24" s="8"/>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -3196,55 +3200,55 @@
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
       <c r="G25" s="10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C26" s="7"/>
       <c r="D26" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
       <c r="G26" s="8"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C27" s="7"/>
       <c r="D27" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
       <c r="G27" s="8"/>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C28" s="7"/>
       <c r="D28" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
       <c r="G28" s="8"/>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -3253,9 +3257,9 @@
       <c r="F29" s="7"/>
       <c r="G29" s="8"/>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -3263,55 +3267,55 @@
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
       <c r="G30" s="10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B31" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="8"/>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B32" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C32" s="7"/>
       <c r="D32" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
       <c r="G32" s="8"/>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B33" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C33" s="7"/>
       <c r="D33" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="8"/>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
@@ -3320,9 +3324,9 @@
       <c r="F34" s="12"/>
       <c r="G34" s="8"/>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -3331,26 +3335,26 @@
       <c r="F35" s="7"/>
       <c r="G35" s="8"/>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B36" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C36" s="7"/>
       <c r="D36" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>0</v>
       </c>
@@ -3359,15 +3363,15 @@
       </c>
       <c r="C37" s="7"/>
       <c r="D37" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F37" s="7"/>
       <c r="G37" s="8"/>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>1</v>
       </c>
@@ -3376,17 +3380,17 @@
       </c>
       <c r="C38" s="7"/>
       <c r="D38" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E38" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F38" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="F38" s="7" t="s">
-        <v>37</v>
-      </c>
       <c r="G38" s="8"/>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>2</v>
       </c>
@@ -3395,15 +3399,15 @@
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F39" s="7"/>
       <c r="G39" s="8"/>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>14</v>
       </c>
@@ -3412,15 +3416,15 @@
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="8"/>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>5</v>
       </c>
@@ -3429,15 +3433,15 @@
       </c>
       <c r="C41" s="7"/>
       <c r="D41" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F41" s="7"/>
       <c r="G41" s="8"/>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>6</v>
       </c>
@@ -3446,34 +3450,34 @@
       </c>
       <c r="C42" s="7"/>
       <c r="D42" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C43" s="7"/>
       <c r="D43" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F43" s="7">
         <v>4</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>3</v>
       </c>
@@ -3482,13 +3486,13 @@
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
       <c r="G44" s="8"/>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>4</v>
       </c>
@@ -3501,9 +3505,9 @@
       <c r="F45" s="7"/>
       <c r="G45" s="8"/>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B46" s="7" t="s">
         <v>10</v>
@@ -3516,9 +3520,9 @@
       </c>
       <c r="G46" s="8"/>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B47" s="7" t="s">
         <v>10</v>
@@ -3526,19 +3530,19 @@
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
       <c r="E47" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F47" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G47" s="8"/>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
@@ -3548,9 +3552,9 @@
       </c>
       <c r="G48" s="8"/>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>11</v>
@@ -3561,12 +3565,12 @@
       <c r="F49" s="7"/>
       <c r="G49" s="8"/>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
@@ -3574,9 +3578,9 @@
       <c r="F50" s="7"/>
       <c r="G50" s="8"/>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>11</v>
@@ -3587,12 +3591,12 @@
       <c r="F51" s="7"/>
       <c r="G51" s="8"/>
     </row>
-    <row r="52" spans="1:7" ht="30">
+    <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
@@ -3601,15 +3605,15 @@
         <v>0</v>
       </c>
       <c r="G52" s="8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="30">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>
@@ -3618,10 +3622,10 @@
         <v>0</v>
       </c>
       <c r="G53" s="8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="8"/>
       <c r="B54" s="13"/>
       <c r="C54" s="7"/>
@@ -3630,41 +3634,30 @@
       <c r="F54" s="7"/>
       <c r="G54" s="8"/>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C55" s="7"/>
-      <c r="D55" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7" t="s">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="G55" s="8"/>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C56" s="7"/>
       <c r="D56" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E56" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="G56" s="8"/>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
         <v>0</v>
       </c>
@@ -3673,68 +3666,68 @@
       </c>
       <c r="C57" s="7"/>
       <c r="D57" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F57" s="7"/>
       <c r="G57" s="8"/>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C58" s="7"/>
-      <c r="D58" s="7"/>
+      <c r="D58" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="E58" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F58" s="7"/>
       <c r="G58" s="8"/>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C59" s="7"/>
       <c r="D59" s="7"/>
       <c r="E59" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F59" s="7" t="b">
-        <v>0</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F59" s="7"/>
       <c r="G59" s="8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
       <c r="E60" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F60" s="7">
-        <v>1</v>
+        <v>35</v>
+      </c>
+      <c r="F60" s="7" t="b">
+        <v>0</v>
       </c>
       <c r="G60" s="8"/>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B61" s="7" t="s">
         <v>10</v>
@@ -3742,16 +3735,16 @@
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F61" s="7" t="b">
-        <v>0</v>
+        <v>35</v>
+      </c>
+      <c r="F61" s="7">
+        <v>1</v>
       </c>
       <c r="G61" s="8"/>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B62" s="7" t="s">
         <v>10</v>
@@ -3759,60 +3752,58 @@
       <c r="C62" s="7"/>
       <c r="D62" s="7"/>
       <c r="E62" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F62" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G62" s="8"/>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>41</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C63" s="7"/>
       <c r="D63" s="7"/>
       <c r="E63" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F63" s="7" t="b">
         <v>0</v>
       </c>
       <c r="G63" s="8"/>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C64" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D64" s="7"/>
       <c r="E64" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F64" s="7">
         <v>0</v>
       </c>
       <c r="G64" s="8"/>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C65" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D65" s="7"/>
       <c r="E65" s="7"/>
@@ -3820,210 +3811,196 @@
         <v>0</v>
       </c>
       <c r="G65" s="8" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7">
-      <c r="A66" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B66" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C66" s="7" t="s">
-        <v>41</v>
-      </c>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B66" s="7"/>
+      <c r="C66" s="7"/>
       <c r="D66" s="7"/>
-      <c r="E66" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F66" s="7">
-        <v>0</v>
-      </c>
+      <c r="E66" s="7"/>
+      <c r="F66" s="7"/>
       <c r="G66" s="8"/>
     </row>
-    <row r="67" spans="1:7">
-      <c r="B67" s="7"/>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="8"/>
+      <c r="B67" s="13"/>
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
       <c r="E67" s="7"/>
       <c r="F67" s="7"/>
       <c r="G67" s="8"/>
     </row>
-    <row r="68" spans="1:7">
-      <c r="A68" s="8"/>
-      <c r="B68" s="13"/>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="C68" s="7"/>
-      <c r="D68" s="7"/>
-      <c r="E68" s="7"/>
-      <c r="F68" s="7"/>
+      <c r="D68" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E68" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F68" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="G68" s="8"/>
     </row>
-    <row r="69" spans="1:7">
-      <c r="A69" s="16" t="s">
-        <v>43</v>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="17" t="s">
+        <v>7</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C69" s="7"/>
       <c r="D69" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F69" s="7" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F69" s="7"/>
       <c r="G69" s="8"/>
     </row>
-    <row r="70" spans="1:7">
-      <c r="A70" s="17" t="s">
-        <v>7</v>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="8" t="s">
+        <v>0</v>
       </c>
       <c r="B70" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C70" s="7"/>
       <c r="D70" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F70" s="7"/>
       <c r="G70" s="8"/>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="8" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C71" s="7"/>
-      <c r="D71" s="7" t="s">
-        <v>59</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="C71" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D71" s="7"/>
       <c r="E71" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F71" s="7"/>
+        <v>35</v>
+      </c>
+      <c r="F71" s="7">
+        <v>1</v>
+      </c>
       <c r="G71" s="8"/>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C72" s="7" t="s">
-        <v>40</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C72" s="7"/>
       <c r="D72" s="7"/>
       <c r="E72" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F72" s="7">
-        <v>1</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F72" s="7"/>
       <c r="G72" s="8"/>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B73" s="7" t="s">
-        <v>11</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B73" s="7"/>
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
-      <c r="E73" s="7" t="s">
-        <v>36</v>
-      </c>
+      <c r="E73" s="7"/>
       <c r="F73" s="7"/>
       <c r="G73" s="8"/>
     </row>
-    <row r="74" spans="1:7">
-      <c r="A74" s="8" t="s">
-        <v>8</v>
-      </c>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="8"/>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
       <c r="D74" s="7"/>
       <c r="E74" s="7"/>
       <c r="F74" s="7"/>
-      <c r="G74" s="8"/>
-    </row>
-    <row r="75" spans="1:7">
-      <c r="A75" s="8"/>
-      <c r="B75" s="7"/>
-      <c r="C75" s="7"/>
-      <c r="D75" s="7"/>
-      <c r="E75" s="7"/>
-      <c r="F75" s="7"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="16" t="s">
+        <v>52</v>
+      </c>
       <c r="G75" s="10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7">
-      <c r="A76" s="16" t="s">
-        <v>53</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="B76" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C76" s="7"/>
       <c r="D76" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E76" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F76" s="7" t="s">
         <v>13</v>
       </c>
       <c r="G76" s="8"/>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B77" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C77" s="7"/>
       <c r="D77" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E77" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F77" s="7"/>
       <c r="G77" s="8"/>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B78" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C78" s="7"/>
       <c r="D78" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E78" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F78" s="7"/>
       <c r="G78" s="8"/>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="B79" s="7" t="s">
         <v>12</v>
@@ -4031,36 +4008,34 @@
       <c r="C79" s="7"/>
       <c r="D79" s="7"/>
       <c r="E79" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F79" s="7"/>
       <c r="G79" s="8"/>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C80" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D80" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E80" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F80" s="7">
         <v>0</v>
       </c>
       <c r="G80" s="8"/>
     </row>
-    <row r="81" spans="1:7">
-      <c r="A81" s="8" t="s">
-        <v>54</v>
-      </c>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="8"/>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
       <c r="D81" s="7"/>
@@ -4068,7 +4043,7 @@
       <c r="F81" s="7"/>
       <c r="G81" s="8"/>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="8"/>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
@@ -4077,46 +4052,50 @@
       <c r="F82" s="7"/>
       <c r="G82" s="8"/>
     </row>
-    <row r="83" spans="1:7">
-      <c r="A83" s="8"/>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="9" t="s">
+        <v>109</v>
+      </c>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
       <c r="D83" s="7"/>
       <c r="E83" s="7"/>
       <c r="F83" s="7"/>
-      <c r="G83" s="8"/>
-    </row>
-    <row r="84" spans="1:7">
-      <c r="A84" s="9" t="s">
+      <c r="G83" s="10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B84" s="7"/>
+      <c r="B84" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="C84" s="7"/>
-      <c r="D84" s="7"/>
-      <c r="E84" s="7"/>
+      <c r="D84" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E84" s="7" t="s">
+        <v>124</v>
+      </c>
       <c r="F84" s="7"/>
-      <c r="G84" s="10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7">
+      <c r="G84" s="8"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="8" t="s">
         <v>111</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C85" s="7"/>
-      <c r="D85" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E85" s="7" t="s">
-        <v>125</v>
-      </c>
+      <c r="D85" s="7"/>
+      <c r="E85" s="7"/>
       <c r="F85" s="7"/>
       <c r="G85" s="8"/>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="8" t="s">
         <v>112</v>
       </c>
@@ -4127,114 +4106,114 @@
       <c r="D86" s="7"/>
       <c r="E86" s="7"/>
       <c r="F86" s="7"/>
-      <c r="G86" s="8"/>
-    </row>
-    <row r="87" spans="1:7">
-      <c r="A87" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="B87" s="7" t="s">
-        <v>11</v>
-      </c>
+      <c r="G86" s="8" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="8"/>
+      <c r="B87" s="7"/>
       <c r="C87" s="7"/>
       <c r="D87" s="7"/>
       <c r="E87" s="7"/>
       <c r="F87" s="7"/>
-      <c r="G87" s="8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7">
-      <c r="A88" s="8"/>
-      <c r="B88" s="7"/>
-      <c r="C88" s="7"/>
-      <c r="D88" s="7"/>
-      <c r="E88" s="7"/>
-      <c r="F88" s="7"/>
+      <c r="G87" s="8"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="9" t="s">
+        <v>65</v>
+      </c>
       <c r="G88" s="8"/>
     </row>
-    <row r="89" spans="1:7">
-      <c r="A89" s="9" t="s">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="8" t="s">
         <v>66</v>
       </c>
+      <c r="B89" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C89" s="7"/>
+      <c r="D89" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E89" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F89" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="G89" s="8"/>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B90" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C90" s="7"/>
       <c r="D90" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E90" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F90" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G90" s="8"/>
-    </row>
-    <row r="91" spans="1:7">
+        <v>35</v>
+      </c>
+      <c r="F90" s="7"/>
+    </row>
+    <row r="91" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A91" s="8" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="B91" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C91" s="7"/>
       <c r="D91" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E91" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F91" s="7"/>
-    </row>
-    <row r="92" spans="1:7" ht="45">
+        <v>35</v>
+      </c>
+      <c r="F91" s="7">
+        <v>1</v>
+      </c>
+      <c r="G91" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B92" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C92" s="7"/>
       <c r="D92" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E92" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F92" s="7">
-        <v>1</v>
-      </c>
-      <c r="G92" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7">
+        <v>35</v>
+      </c>
+      <c r="F92" s="7"/>
+      <c r="G92" s="8"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="8" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B93" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C93" s="7"/>
-      <c r="D93" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="E93" s="7" t="s">
-        <v>36</v>
-      </c>
+      <c r="D93" s="7"/>
+      <c r="E93" s="7"/>
       <c r="F93" s="7"/>
       <c r="G93" s="8"/>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="8" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="B94" s="7" t="s">
         <v>11</v>
@@ -4245,12 +4224,12 @@
       <c r="F94" s="7"/>
       <c r="G94" s="8"/>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="8" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C95" s="7"/>
       <c r="D95" s="7"/>
@@ -4258,9 +4237,9 @@
       <c r="F95" s="7"/>
       <c r="G95" s="8"/>
     </row>
-    <row r="96" spans="1:7">
-      <c r="A96" s="8" t="s">
-        <v>74</v>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A96" s="17" t="s">
+        <v>78</v>
       </c>
       <c r="B96" s="7" t="s">
         <v>12</v>
@@ -4271,9 +4250,9 @@
       <c r="F96" s="7"/>
       <c r="G96" s="8"/>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="17" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B97" s="7" t="s">
         <v>12</v>
@@ -4284,9 +4263,9 @@
       <c r="F97" s="7"/>
       <c r="G97" s="8"/>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="17" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B98" s="7" t="s">
         <v>12</v>
@@ -4297,9 +4276,9 @@
       <c r="F98" s="7"/>
       <c r="G98" s="8"/>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="17" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="B99" s="7" t="s">
         <v>12</v>
@@ -4308,26 +4287,26 @@
       <c r="D99" s="7"/>
       <c r="E99" s="7"/>
       <c r="F99" s="7"/>
-      <c r="G99" s="8"/>
-    </row>
-    <row r="100" spans="1:7">
-      <c r="A100" s="17" t="s">
-        <v>100</v>
+      <c r="G99" s="8" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="8" t="s">
+        <v>70</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C100" s="7"/>
       <c r="D100" s="7"/>
       <c r="E100" s="7"/>
       <c r="F100" s="7"/>
-      <c r="G100" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7">
+      <c r="G100" s="8"/>
+    </row>
+    <row r="101" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
-        <v>71</v>
+        <v>125</v>
       </c>
       <c r="B101" s="7" t="s">
         <v>11</v>
@@ -4336,197 +4315,193 @@
       <c r="D101" s="7"/>
       <c r="E101" s="7"/>
       <c r="F101" s="7"/>
-      <c r="G101" s="8"/>
-    </row>
-    <row r="102" spans="1:7" ht="45">
+      <c r="G101" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="8" t="s">
-        <v>126</v>
+        <v>189</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C102" s="7"/>
+        <v>15</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="D102" s="7"/>
       <c r="E102" s="7"/>
-      <c r="F102" s="7"/>
+      <c r="F102" s="7">
+        <v>0</v>
+      </c>
       <c r="G102" s="8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7">
-      <c r="A103" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="B103" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C103" s="7" t="s">
-        <v>41</v>
-      </c>
+        <v>188</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="8"/>
+      <c r="B103" s="7"/>
+      <c r="C103" s="7"/>
       <c r="D103" s="7"/>
       <c r="E103" s="7"/>
-      <c r="F103" s="7">
-        <v>0</v>
-      </c>
-      <c r="G103" s="8" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7">
-      <c r="A104" s="8"/>
+      <c r="F103" s="7"/>
+      <c r="G103" s="8"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="9" t="s">
+        <v>102</v>
+      </c>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
       <c r="D104" s="7"/>
       <c r="E104" s="7"/>
       <c r="F104" s="7"/>
-      <c r="G104" s="8"/>
-    </row>
-    <row r="105" spans="1:7">
-      <c r="A105" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="B105" s="7"/>
+      <c r="G104" s="10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B105" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="C105" s="7"/>
-      <c r="D105" s="7"/>
+      <c r="D105" s="7" t="s">
+        <v>59</v>
+      </c>
       <c r="E105" s="7"/>
       <c r="F105" s="7"/>
-      <c r="G105" s="10" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7">
-      <c r="A106" s="18" t="s">
-        <v>7</v>
+      <c r="G105" s="17"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="8" t="s">
+        <v>103</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C106" s="7"/>
       <c r="D106" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E106" s="7"/>
+        <v>57</v>
+      </c>
+      <c r="E106" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="F106" s="7"/>
-      <c r="G106" s="17"/>
-    </row>
-    <row r="107" spans="1:7">
+      <c r="G106" s="8"/>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="8" t="s">
-        <v>104</v>
+        <v>66</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C107" s="7"/>
       <c r="D107" s="7" t="s">
         <v>58</v>
       </c>
       <c r="E107" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F107" s="7"/>
       <c r="G107" s="8"/>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="8" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="B108" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C108" s="7"/>
       <c r="D108" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E108" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F108" s="7"/>
       <c r="G108" s="8"/>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="8" t="s">
         <v>105</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C109" s="7"/>
       <c r="D109" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E109" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F109" s="7"/>
       <c r="G109" s="8"/>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="8" t="s">
         <v>106</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>11</v>
+        <v>96</v>
       </c>
       <c r="C110" s="7"/>
-      <c r="D110" s="7" t="s">
-        <v>59</v>
-      </c>
+      <c r="D110" s="7"/>
       <c r="E110" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F110" s="7"/>
       <c r="G110" s="8"/>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C111" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D111" s="7"/>
+      <c r="E111" s="7"/>
+      <c r="F111" s="7">
+        <v>0</v>
+      </c>
+      <c r="G111" s="8"/>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B111" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C111" s="7"/>
-      <c r="D111" s="7"/>
-      <c r="E111" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F111" s="7"/>
-      <c r="G111" s="8"/>
-    </row>
-    <row r="112" spans="1:7">
-      <c r="A112" s="8" t="s">
-        <v>109</v>
-      </c>
       <c r="B112" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C112" s="7" t="s">
-        <v>47</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="C112" s="7"/>
       <c r="D112" s="7"/>
-      <c r="E112" s="7"/>
-      <c r="F112" s="7">
-        <v>0</v>
+      <c r="E112" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F112" s="7" t="b">
+        <v>1</v>
       </c>
       <c r="G112" s="8"/>
     </row>
-    <row r="113" spans="1:7">
-      <c r="A113" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="B113" s="7" t="s">
-        <v>10</v>
-      </c>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="8"/>
+      <c r="B113" s="7"/>
       <c r="C113" s="7"/>
       <c r="D113" s="7"/>
-      <c r="E113" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F113" s="7" t="b">
-        <v>1</v>
-      </c>
+      <c r="E113" s="7"/>
+      <c r="F113" s="7"/>
       <c r="G113" s="8"/>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="8"/>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
@@ -4535,8 +4510,10 @@
       <c r="F114" s="7"/>
       <c r="G114" s="8"/>
     </row>
-    <row r="115" spans="1:7">
-      <c r="A115" s="8"/>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" s="16" t="s">
+        <v>90</v>
+      </c>
       <c r="B115" s="7"/>
       <c r="C115" s="7"/>
       <c r="D115" s="7"/>
@@ -4544,18 +4521,24 @@
       <c r="F115" s="7"/>
       <c r="G115" s="8"/>
     </row>
-    <row r="116" spans="1:7">
-      <c r="A116" s="16" t="s">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="B116" s="7"/>
+      <c r="B116" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="C116" s="7"/>
-      <c r="D116" s="7"/>
-      <c r="E116" s="7"/>
+      <c r="D116" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E116" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="F116" s="7"/>
       <c r="G116" s="8"/>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="8" t="s">
         <v>92</v>
       </c>
@@ -4564,166 +4547,160 @@
       </c>
       <c r="C117" s="7"/>
       <c r="D117" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E117" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F117" s="7"/>
       <c r="G117" s="8"/>
     </row>
-    <row r="118" spans="1:7">
-      <c r="A118" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B118" s="7" t="s">
-        <v>11</v>
-      </c>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" s="8"/>
+      <c r="B118" s="7"/>
       <c r="C118" s="7"/>
-      <c r="D118" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E118" s="7" t="s">
-        <v>36</v>
-      </c>
+      <c r="D118" s="7"/>
+      <c r="E118" s="7"/>
       <c r="F118" s="7"/>
       <c r="G118" s="8"/>
     </row>
-    <row r="119" spans="1:7">
-      <c r="A119" s="8"/>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" s="16" t="s">
+        <v>93</v>
+      </c>
       <c r="B119" s="7"/>
       <c r="C119" s="7"/>
       <c r="D119" s="7"/>
       <c r="E119" s="7"/>
       <c r="F119" s="7"/>
-      <c r="G119" s="8"/>
-    </row>
-    <row r="120" spans="1:7">
-      <c r="A120" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="B120" s="7"/>
+      <c r="G119" s="8" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="C120" s="7"/>
-      <c r="D120" s="7"/>
-      <c r="E120" s="7"/>
+      <c r="D120" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E120" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="F120" s="7"/>
-      <c r="G120" s="8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="121" spans="1:7">
+      <c r="G120" s="8"/>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="8" t="s">
-        <v>7</v>
+        <v>91</v>
       </c>
       <c r="B121" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C121" s="7"/>
       <c r="D121" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E121" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F121" s="7"/>
       <c r="G121" s="8"/>
     </row>
-    <row r="122" spans="1:7">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="8" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B122" s="7" t="s">
-        <v>11</v>
+        <v>96</v>
       </c>
       <c r="C122" s="7"/>
       <c r="D122" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E122" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F122" s="7"/>
       <c r="G122" s="8"/>
     </row>
-    <row r="123" spans="1:7">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="8" t="s">
         <v>95</v>
       </c>
       <c r="B123" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C123" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="C123" s="7"/>
-      <c r="D123" s="7" t="s">
-        <v>59</v>
-      </c>
+      <c r="D123" s="7"/>
       <c r="E123" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F123" s="7"/>
+        <v>35</v>
+      </c>
+      <c r="F123" s="7">
+        <v>0</v>
+      </c>
       <c r="G123" s="8"/>
     </row>
-    <row r="124" spans="1:7">
-      <c r="A124" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="B124" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C124" s="7" t="s">
-        <v>98</v>
-      </c>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" s="8"/>
+      <c r="B124" s="7"/>
+      <c r="C124" s="7"/>
       <c r="D124" s="7"/>
-      <c r="E124" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F124" s="7">
-        <v>0</v>
-      </c>
+      <c r="E124" s="7"/>
+      <c r="F124" s="7"/>
       <c r="G124" s="8"/>
     </row>
-    <row r="125" spans="1:7">
-      <c r="A125" s="8"/>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" s="9" t="s">
+        <v>116</v>
+      </c>
       <c r="B125" s="7"/>
       <c r="C125" s="7"/>
       <c r="D125" s="7"/>
       <c r="E125" s="7"/>
       <c r="F125" s="7"/>
-      <c r="G125" s="8"/>
-    </row>
-    <row r="126" spans="1:7">
-      <c r="A126" s="9" t="s">
+      <c r="G125" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A126" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="B126" s="7"/>
+      <c r="B126" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="C126" s="7"/>
-      <c r="D126" s="7"/>
-      <c r="E126" s="7"/>
+      <c r="D126" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E126" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="F126" s="7"/>
-      <c r="G126" s="10" t="s">
+      <c r="G126" s="8" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="127" spans="1:7" ht="45">
-      <c r="A127" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B127" s="7" t="s">
-        <v>11</v>
-      </c>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127" s="8"/>
+      <c r="B127" s="7"/>
       <c r="C127" s="7"/>
-      <c r="D127" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E127" s="7" t="s">
-        <v>36</v>
-      </c>
+      <c r="D127" s="7"/>
+      <c r="E127" s="7"/>
       <c r="F127" s="7"/>
-      <c r="G127" s="8" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7">
-      <c r="A128" s="8"/>
+      <c r="G127" s="8"/>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" s="9" t="s">
+        <v>131</v>
+      </c>
       <c r="B128" s="7"/>
       <c r="C128" s="7"/>
       <c r="D128" s="7"/>
@@ -4731,52 +4708,58 @@
       <c r="F128" s="7"/>
       <c r="G128" s="8"/>
     </row>
-    <row r="129" spans="1:7">
-      <c r="A129" s="9" t="s">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129" s="8" t="s">
         <v>132</v>
       </c>
-      <c r="B129" s="7"/>
+      <c r="B129" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="C129" s="7"/>
-      <c r="D129" s="7"/>
-      <c r="E129" s="7"/>
+      <c r="D129" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E129" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="F129" s="7"/>
       <c r="G129" s="8"/>
     </row>
-    <row r="130" spans="1:7">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="8" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B130" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C130" s="7"/>
       <c r="D130" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E130" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F130" s="7"/>
       <c r="G130" s="8"/>
     </row>
-    <row r="131" spans="1:7">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="8" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B131" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C131" s="7"/>
       <c r="D131" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E131" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F131" s="7"/>
       <c r="G131" s="8"/>
     </row>
-    <row r="132" spans="1:7">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="8" t="s">
         <v>134</v>
       </c>
@@ -4784,16 +4767,16 @@
         <v>11</v>
       </c>
       <c r="C132" s="7"/>
-      <c r="D132" s="7" t="s">
-        <v>58</v>
-      </c>
+      <c r="D132" s="7"/>
       <c r="E132" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F132" s="7"/>
-      <c r="G132" s="8"/>
-    </row>
-    <row r="133" spans="1:7">
+      <c r="G132" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="8" t="s">
         <v>135</v>
       </c>
@@ -4801,36 +4784,30 @@
         <v>11</v>
       </c>
       <c r="C133" s="7"/>
-      <c r="D133" s="7"/>
+      <c r="D133" s="7" t="s">
+        <v>58</v>
+      </c>
       <c r="E133" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F133" s="7"/>
       <c r="G133" s="8" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="134" spans="1:7">
-      <c r="A134" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="B134" s="7" t="s">
-        <v>11</v>
-      </c>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134" s="8"/>
+      <c r="B134" s="7"/>
       <c r="C134" s="7"/>
-      <c r="D134" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E134" s="7" t="s">
-        <v>36</v>
-      </c>
+      <c r="D134" s="7"/>
+      <c r="E134" s="7"/>
       <c r="F134" s="7"/>
-      <c r="G134" s="8" t="s">
+      <c r="G134" s="8"/>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135" s="9" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="135" spans="1:7">
-      <c r="A135" s="8"/>
       <c r="B135" s="7"/>
       <c r="C135" s="7"/>
       <c r="D135" s="7"/>
@@ -4838,52 +4815,58 @@
       <c r="F135" s="7"/>
       <c r="G135" s="8"/>
     </row>
-    <row r="136" spans="1:7">
-      <c r="A136" s="9" t="s">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="B136" s="7"/>
+      <c r="B136" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="C136" s="7"/>
-      <c r="D136" s="7"/>
-      <c r="E136" s="7"/>
+      <c r="D136" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E136" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="F136" s="7"/>
       <c r="G136" s="8"/>
     </row>
-    <row r="137" spans="1:7">
-      <c r="A137" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="B137" s="7" t="s">
-        <v>11</v>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="B137" s="14" t="s">
+        <v>12</v>
       </c>
       <c r="C137" s="7"/>
       <c r="D137" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E137" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F137" s="7"/>
       <c r="G137" s="8"/>
     </row>
-    <row r="138" spans="1:7">
-      <c r="A138" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="B138" s="14" t="s">
-        <v>12</v>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B138" s="7" t="s">
+        <v>11</v>
       </c>
       <c r="C138" s="7"/>
       <c r="D138" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E138" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F138" s="7"/>
       <c r="G138" s="8"/>
     </row>
-    <row r="139" spans="1:7">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="8" t="s">
         <v>142</v>
       </c>
@@ -4895,84 +4878,84 @@
         <v>58</v>
       </c>
       <c r="E139" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F139" s="7"/>
-      <c r="G139" s="8"/>
-    </row>
-    <row r="140" spans="1:7">
+      <c r="G139" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="8" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B140" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C140" s="7"/>
       <c r="D140" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E140" s="7" t="s">
-        <v>36</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="E140" s="7"/>
       <c r="F140" s="7"/>
       <c r="G140" s="8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="8" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B141" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C141" s="7"/>
-      <c r="D141" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E141" s="7"/>
+      <c r="D141" s="7"/>
+      <c r="E141" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="F141" s="7"/>
       <c r="G141" s="8" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="142" spans="1:7">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="8" t="s">
-        <v>147</v>
+        <v>91</v>
       </c>
       <c r="B142" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C142" s="7"/>
       <c r="D142" s="7"/>
       <c r="E142" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F142" s="7"/>
       <c r="G142" s="8" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="8" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="B143" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C143" s="7"/>
       <c r="D143" s="7"/>
       <c r="E143" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F143" s="7"/>
-      <c r="G143" s="8" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7">
+        <v>35</v>
+      </c>
+      <c r="F143" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G143" s="8"/>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="8" t="s">
-        <v>108</v>
+        <v>148</v>
       </c>
       <c r="B144" s="7" t="s">
         <v>10</v>
@@ -4980,33 +4963,25 @@
       <c r="C144" s="7"/>
       <c r="D144" s="7"/>
       <c r="E144" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F144" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G144" s="8"/>
-    </row>
-    <row r="145" spans="1:7">
-      <c r="A145" s="8" t="s">
+      <c r="G144" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="B145" s="7" t="s">
-        <v>10</v>
-      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145" s="8"/>
+      <c r="B145" s="7"/>
       <c r="C145" s="7"/>
       <c r="D145" s="7"/>
-      <c r="E145" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F145" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G145" s="8" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="146" spans="1:7">
+      <c r="E145" s="7"/>
+      <c r="F145" s="7"/>
+      <c r="G145" s="8"/>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="8"/>
       <c r="B146" s="7"/>
       <c r="C146" s="7"/>
@@ -5015,7 +4990,7 @@
       <c r="F146" s="7"/>
       <c r="G146" s="8"/>
     </row>
-    <row r="147" spans="1:7">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="8"/>
       <c r="B147" s="7"/>
       <c r="C147" s="7"/>
@@ -5024,8 +4999,10 @@
       <c r="F147" s="7"/>
       <c r="G147" s="8"/>
     </row>
-    <row r="148" spans="1:7">
-      <c r="A148" s="8"/>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A148" s="9" t="s">
+        <v>158</v>
+      </c>
       <c r="B148" s="7"/>
       <c r="C148" s="7"/>
       <c r="D148" s="7"/>
@@ -5033,56 +5010,58 @@
       <c r="F148" s="7"/>
       <c r="G148" s="8"/>
     </row>
-    <row r="149" spans="1:7">
-      <c r="A149" s="9" t="s">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A149" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="B149" s="7"/>
+      <c r="B149" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="C149" s="7"/>
-      <c r="D149" s="7"/>
-      <c r="E149" s="7"/>
-      <c r="F149" s="7"/>
+      <c r="D149" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E149" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F149" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="G149" s="8"/>
     </row>
-    <row r="150" spans="1:7">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="8" t="s">
         <v>160</v>
       </c>
       <c r="B150" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C150" s="7"/>
       <c r="D150" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E150" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F150" s="7" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F150" s="7"/>
       <c r="G150" s="8"/>
     </row>
-    <row r="151" spans="1:7">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="8" t="s">
-        <v>161</v>
+        <v>71</v>
       </c>
       <c r="B151" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C151" s="7"/>
-      <c r="D151" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E151" s="7" t="s">
-        <v>36</v>
-      </c>
+      <c r="D151" s="7"/>
+      <c r="E151" s="7"/>
       <c r="F151" s="7"/>
       <c r="G151" s="8"/>
     </row>
-    <row r="152" spans="1:7">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="8" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="B152" s="7" t="s">
         <v>11</v>
@@ -5093,12 +5072,12 @@
       <c r="F152" s="7"/>
       <c r="G152" s="8"/>
     </row>
-    <row r="153" spans="1:7">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="8" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="B153" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C153" s="7"/>
       <c r="D153" s="7"/>
@@ -5106,9 +5085,9 @@
       <c r="F153" s="7"/>
       <c r="G153" s="8"/>
     </row>
-    <row r="154" spans="1:7">
-      <c r="A154" s="8" t="s">
-        <v>74</v>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A154" s="17" t="s">
+        <v>78</v>
       </c>
       <c r="B154" s="7" t="s">
         <v>12</v>
@@ -5119,9 +5098,9 @@
       <c r="F154" s="7"/>
       <c r="G154" s="8"/>
     </row>
-    <row r="155" spans="1:7">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="17" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B155" s="7" t="s">
         <v>12</v>
@@ -5132,9 +5111,9 @@
       <c r="F155" s="7"/>
       <c r="G155" s="8"/>
     </row>
-    <row r="156" spans="1:7">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="17" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B156" s="7" t="s">
         <v>12</v>
@@ -5145,101 +5124,105 @@
       <c r="F156" s="7"/>
       <c r="G156" s="8"/>
     </row>
-    <row r="157" spans="1:7">
-      <c r="A157" s="17" t="s">
-        <v>85</v>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A157" s="8" t="s">
+        <v>202</v>
       </c>
       <c r="B157" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C157" s="7"/>
       <c r="D157" s="7"/>
-      <c r="E157" s="7"/>
-      <c r="F157" s="7"/>
-      <c r="G157" s="8"/>
-    </row>
-    <row r="158" spans="1:7">
-      <c r="A158" s="8" t="s">
+      <c r="E157" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F157" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G157" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="B158" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C158" s="7"/>
-      <c r="D158" s="7"/>
-      <c r="E158" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F158" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G158" s="8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="160" spans="1:7">
-      <c r="A160" s="9" t="s">
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A159" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="B159" s="7"/>
+      <c r="C159" s="7"/>
+      <c r="D159" s="7"/>
+      <c r="E159" s="7"/>
+      <c r="F159" s="7"/>
+      <c r="G159" s="8"/>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A160" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="B160" s="7"/>
+      <c r="B160" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="C160" s="7"/>
-      <c r="D160" s="7"/>
-      <c r="E160" s="7"/>
-      <c r="F160" s="7"/>
+      <c r="D160" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E160" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F160" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="G160" s="8"/>
     </row>
-    <row r="161" spans="1:7">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="8" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B161" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C161" s="7"/>
       <c r="D161" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E161" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F161" s="7" t="s">
-        <v>13</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="F161" s="7"/>
       <c r="G161" s="8"/>
     </row>
-    <row r="162" spans="1:7">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="8" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B162" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C162" s="7"/>
-      <c r="D162" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E162" s="7" t="s">
-        <v>36</v>
-      </c>
+      <c r="D162" s="7"/>
+      <c r="E162" s="7"/>
       <c r="F162" s="7"/>
       <c r="G162" s="8"/>
     </row>
-    <row r="163" spans="1:7">
+    <row r="163" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" s="8" t="s">
         <v>162</v>
       </c>
       <c r="B163" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C163" s="7"/>
       <c r="D163" s="7"/>
       <c r="E163" s="7"/>
-      <c r="F163" s="7"/>
-      <c r="G163" s="8"/>
-    </row>
-    <row r="164" spans="1:7" ht="30">
+      <c r="F163" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="G163" s="8" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="8" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="B164" s="7" t="s">
         <v>10</v>
@@ -5251,27 +5234,19 @@
         <v>0</v>
       </c>
       <c r="G164" s="8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="165" spans="1:7">
-      <c r="A165" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="B165" s="7" t="s">
-        <v>10</v>
-      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A165" s="8"/>
+      <c r="B165" s="7"/>
       <c r="C165" s="7"/>
       <c r="D165" s="7"/>
       <c r="E165" s="7"/>
-      <c r="F165" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="G165" s="8" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="166" spans="1:7">
+      <c r="F165" s="7"/>
+      <c r="G165" s="8"/>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="8"/>
       <c r="B166" s="7"/>
       <c r="C166" s="7"/>
@@ -5280,7 +5255,7 @@
       <c r="F166" s="7"/>
       <c r="G166" s="8"/>
     </row>
-    <row r="167" spans="1:7">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="8"/>
       <c r="B167" s="7"/>
       <c r="C167" s="7"/>
@@ -5289,7 +5264,7 @@
       <c r="F167" s="7"/>
       <c r="G167" s="8"/>
     </row>
-    <row r="168" spans="1:7">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="8"/>
       <c r="B168" s="7"/>
       <c r="C168" s="7"/>
@@ -5298,7 +5273,7 @@
       <c r="F168" s="7"/>
       <c r="G168" s="8"/>
     </row>
-    <row r="169" spans="1:7">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="8"/>
       <c r="B169" s="7"/>
       <c r="C169" s="7"/>
@@ -5307,7 +5282,7 @@
       <c r="F169" s="7"/>
       <c r="G169" s="8"/>
     </row>
-    <row r="170" spans="1:7">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="8"/>
       <c r="B170" s="7"/>
       <c r="C170" s="7"/>
@@ -5316,7 +5291,7 @@
       <c r="F170" s="7"/>
       <c r="G170" s="8"/>
     </row>
-    <row r="171" spans="1:7">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="8"/>
       <c r="B171" s="7"/>
       <c r="C171" s="7"/>
@@ -5325,7 +5300,7 @@
       <c r="F171" s="7"/>
       <c r="G171" s="8"/>
     </row>
-    <row r="172" spans="1:7">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="8"/>
       <c r="B172" s="7"/>
       <c r="C172" s="7"/>
@@ -5334,7 +5309,7 @@
       <c r="F172" s="7"/>
       <c r="G172" s="8"/>
     </row>
-    <row r="173" spans="1:7">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="8"/>
       <c r="B173" s="7"/>
       <c r="C173" s="7"/>
@@ -5343,7 +5318,7 @@
       <c r="F173" s="7"/>
       <c r="G173" s="8"/>
     </row>
-    <row r="174" spans="1:7">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="8"/>
       <c r="B174" s="7"/>
       <c r="C174" s="7"/>
@@ -5352,7 +5327,7 @@
       <c r="F174" s="7"/>
       <c r="G174" s="8"/>
     </row>
-    <row r="175" spans="1:7">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="8"/>
       <c r="B175" s="7"/>
       <c r="C175" s="7"/>
@@ -5361,7 +5336,7 @@
       <c r="F175" s="7"/>
       <c r="G175" s="8"/>
     </row>
-    <row r="176" spans="1:7">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="8"/>
       <c r="B176" s="7"/>
       <c r="C176" s="7"/>
@@ -5370,7 +5345,7 @@
       <c r="F176" s="7"/>
       <c r="G176" s="8"/>
     </row>
-    <row r="177" spans="1:7">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="8"/>
       <c r="B177" s="7"/>
       <c r="C177" s="7"/>
@@ -5379,7 +5354,7 @@
       <c r="F177" s="7"/>
       <c r="G177" s="8"/>
     </row>
-    <row r="178" spans="1:7">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="8"/>
       <c r="B178" s="7"/>
       <c r="C178" s="7"/>
@@ -5388,7 +5363,7 @@
       <c r="F178" s="7"/>
       <c r="G178" s="8"/>
     </row>
-    <row r="179" spans="1:7">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="8"/>
       <c r="B179" s="7"/>
       <c r="C179" s="7"/>
@@ -5397,7 +5372,7 @@
       <c r="F179" s="7"/>
       <c r="G179" s="8"/>
     </row>
-    <row r="180" spans="1:7">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="8"/>
       <c r="B180" s="7"/>
       <c r="C180" s="7"/>
@@ -5406,7 +5381,7 @@
       <c r="F180" s="7"/>
       <c r="G180" s="8"/>
     </row>
-    <row r="181" spans="1:7">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="8"/>
       <c r="B181" s="7"/>
       <c r="C181" s="7"/>
@@ -5415,7 +5390,7 @@
       <c r="F181" s="7"/>
       <c r="G181" s="8"/>
     </row>
-    <row r="182" spans="1:7">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="8"/>
       <c r="B182" s="7"/>
       <c r="C182" s="7"/>
@@ -5424,7 +5399,7 @@
       <c r="F182" s="7"/>
       <c r="G182" s="8"/>
     </row>
-    <row r="183" spans="1:7">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="8"/>
       <c r="B183" s="7"/>
       <c r="C183" s="7"/>
@@ -5433,7 +5408,7 @@
       <c r="F183" s="7"/>
       <c r="G183" s="8"/>
     </row>
-    <row r="184" spans="1:7">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="8"/>
       <c r="B184" s="7"/>
       <c r="C184" s="7"/>
@@ -5442,7 +5417,7 @@
       <c r="F184" s="7"/>
       <c r="G184" s="8"/>
     </row>
-    <row r="185" spans="1:7">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="8"/>
       <c r="B185" s="7"/>
       <c r="C185" s="7"/>
@@ -5451,7 +5426,7 @@
       <c r="F185" s="7"/>
       <c r="G185" s="8"/>
     </row>
-    <row r="186" spans="1:7">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="8"/>
       <c r="B186" s="7"/>
       <c r="C186" s="7"/>
@@ -5460,7 +5435,7 @@
       <c r="F186" s="7"/>
       <c r="G186" s="8"/>
     </row>
-    <row r="187" spans="1:7">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="8"/>
       <c r="B187" s="7"/>
       <c r="C187" s="7"/>
@@ -5469,7 +5444,7 @@
       <c r="F187" s="7"/>
       <c r="G187" s="8"/>
     </row>
-    <row r="188" spans="1:7">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="8"/>
       <c r="B188" s="7"/>
       <c r="C188" s="7"/>
@@ -5478,7 +5453,7 @@
       <c r="F188" s="7"/>
       <c r="G188" s="8"/>
     </row>
-    <row r="189" spans="1:7">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="8"/>
       <c r="B189" s="7"/>
       <c r="C189" s="7"/>
@@ -5487,7 +5462,7 @@
       <c r="F189" s="7"/>
       <c r="G189" s="8"/>
     </row>
-    <row r="190" spans="1:7">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="8"/>
       <c r="B190" s="7"/>
       <c r="C190" s="7"/>
@@ -5496,7 +5471,7 @@
       <c r="F190" s="7"/>
       <c r="G190" s="8"/>
     </row>
-    <row r="191" spans="1:7">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="8"/>
       <c r="B191" s="7"/>
       <c r="C191" s="7"/>
@@ -5505,7 +5480,7 @@
       <c r="F191" s="7"/>
       <c r="G191" s="8"/>
     </row>
-    <row r="192" spans="1:7">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="8"/>
       <c r="B192" s="7"/>
       <c r="C192" s="7"/>
@@ -5514,7 +5489,7 @@
       <c r="F192" s="7"/>
       <c r="G192" s="8"/>
     </row>
-    <row r="193" spans="1:7">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" s="8"/>
       <c r="B193" s="7"/>
       <c r="C193" s="7"/>
@@ -5523,7 +5498,7 @@
       <c r="F193" s="7"/>
       <c r="G193" s="8"/>
     </row>
-    <row r="194" spans="1:7">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="8"/>
       <c r="B194" s="7"/>
       <c r="C194" s="7"/>
@@ -5532,7 +5507,7 @@
       <c r="F194" s="7"/>
       <c r="G194" s="8"/>
     </row>
-    <row r="195" spans="1:7">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" s="8"/>
       <c r="B195" s="7"/>
       <c r="C195" s="7"/>
@@ -5541,7 +5516,7 @@
       <c r="F195" s="7"/>
       <c r="G195" s="8"/>
     </row>
-    <row r="196" spans="1:7">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" s="8"/>
       <c r="B196" s="7"/>
       <c r="C196" s="7"/>
@@ -5550,7 +5525,7 @@
       <c r="F196" s="7"/>
       <c r="G196" s="8"/>
     </row>
-    <row r="197" spans="1:7">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" s="8"/>
       <c r="B197" s="7"/>
       <c r="C197" s="7"/>
@@ -5559,7 +5534,7 @@
       <c r="F197" s="7"/>
       <c r="G197" s="8"/>
     </row>
-    <row r="198" spans="1:7">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" s="8"/>
       <c r="B198" s="7"/>
       <c r="C198" s="7"/>
@@ -5568,7 +5543,7 @@
       <c r="F198" s="7"/>
       <c r="G198" s="8"/>
     </row>
-    <row r="199" spans="1:7">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" s="8"/>
       <c r="B199" s="7"/>
       <c r="C199" s="7"/>
@@ -5577,15 +5552,6 @@
       <c r="F199" s="7"/>
       <c r="G199" s="8"/>
     </row>
-    <row r="200" spans="1:7">
-      <c r="A200" s="8"/>
-      <c r="B200" s="7"/>
-      <c r="C200" s="7"/>
-      <c r="D200" s="7"/>
-      <c r="E200" s="7"/>
-      <c r="F200" s="7"/>
-      <c r="G200" s="8"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5593,53 +5559,53 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="I2:N35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="Q50" sqref="Q50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="14:14">
+    <row r="2" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N4" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="4" spans="14:14">
-      <c r="N4" t="s">
+    <row r="5" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N5" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="5" spans="14:14">
-      <c r="N5" t="s">
+    <row r="6" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N6" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="6" spans="14:14">
-      <c r="N6" t="s">
+    <row r="7" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N7" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="7" spans="14:14">
-      <c r="N7" t="s">
+    <row r="8" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N8" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="8" spans="14:14">
-      <c r="N8" t="s">
+    <row r="10" spans="14:14" x14ac:dyDescent="0.25">
+      <c r="N10" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="10" spans="14:14">
-      <c r="N10" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="35" spans="9:9">
-      <c r="I35" s="24" t="s">
-        <v>205</v>
+    <row r="35" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I35" s="23" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -5650,14 +5616,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="3" width="9.140625" style="19"/>
@@ -5667,37 +5633,37 @@
     <col min="7" max="7" width="98" style="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="45.75" customHeight="1">
+    <row r="1" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>153</v>
       </c>
       <c r="B4" s="19" t="s">
         <v>11</v>
@@ -5706,106 +5672,106 @@
         <v>20</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="19" t="s">
         <v>154</v>
       </c>
-      <c r="B5" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="19" t="s">
         <v>12</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G6" s="21" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B7" s="19" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B8" s="19" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="G8" s="22" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>58</v>
+      </c>
+      <c r="G8" s="24" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B9" s="19" t="s">
         <v>12</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="G9" s="22"/>
-    </row>
-    <row r="10" spans="1:7">
+        <v>58</v>
+      </c>
+      <c r="G9" s="24"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B10" s="19" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>59</v>
-      </c>
-      <c r="G10" s="22"/>
-    </row>
-    <row r="11" spans="1:7">
+        <v>58</v>
+      </c>
+      <c r="G10" s="24"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B12" s="19" t="s">
         <v>10</v>
@@ -5814,12 +5780,12 @@
         <v>0</v>
       </c>
       <c r="G12" s="21" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B13" s="19" t="s">
         <v>10</v>
@@ -5828,80 +5794,80 @@
         <v>1</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F14" s="19">
         <v>0</v>
       </c>
       <c r="G14" s="21" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F15" s="19">
         <v>0</v>
       </c>
       <c r="G15" s="21" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F16" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F17" s="19">
         <v>0</v>
       </c>
       <c r="G17" s="21" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -5909,133 +5875,133 @@
         <v>12</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E20" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F20" s="19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B21" s="19" t="s">
         <v>11</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B22" s="19" t="s">
         <v>12</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F22" s="19" t="s">
         <v>13</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B23" s="19" t="s">
         <v>12</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F24" s="19">
         <v>1</v>
       </c>
       <c r="G24" s="21" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" t="s">
-        <v>182</v>
-      </c>
       <c r="B25" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F25" s="19">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B26" s="19" t="s">
         <v>11</v>
       </c>
       <c r="G26" s="21" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="G29" s="23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G29" s="22" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G30" s="21" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="30">
-      <c r="G30" s="21" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="30">
+    <row r="31" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="G31" s="21" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G32" s="21" t="s">
         <v>194</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="30">
-      <c r="G32" s="21" t="s">
-        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>